<commit_message>
[paper1] Add and modify input data
* Add the data from the original paper of the experiment.

* Create a larsa moment curvature data from the material properties mentioned in the original experiment.
</commit_message>
<xml_diff>
--- a/Models/paper1/frame.xlsx
+++ b/Models/paper1/frame.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Coordinates" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,11 +15,8 @@
     <sheet name="Materials" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Sections" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="Nodal Load" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="curve1" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="T1Ma" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="curve2" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="24 element" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="E0greaterEcr" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="E0equalEcr" sheetId="12" state="visible" r:id="rId13"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -31,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
   <si>
     <t xml:space="preserve">Node ID</t>
   </si>
@@ -141,7 +138,7 @@
     <t xml:space="preserve">Moment Curvature Curve Sheet Name</t>
   </si>
   <si>
-    <t xml:space="preserve">curve2</t>
+    <t xml:space="preserve">T1Ma</t>
   </si>
   <si>
     <t xml:space="preserve">Load ID</t>
@@ -159,19 +156,16 @@
     <t xml:space="preserve">Fz</t>
   </si>
   <si>
+    <t xml:space="preserve">rad/m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">knm</t>
+  </si>
+  <si>
     <t xml:space="preserve">Curvature</t>
   </si>
   <si>
     <t xml:space="preserve">Moment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24 element</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E0 &gt; ecr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E0 = ecr</t>
   </si>
 </sst>
 </file>
@@ -182,7 +176,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -211,18 +205,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="162"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF595959"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF595959"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -329,7 +311,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFBFBFBF"/>
+      <rgbColor rgb="FFB3B3B3"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -338,7 +320,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFD9D9D9"/>
+      <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -355,14 +337,14 @@
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF4472C4"/>
+      <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF595959"/>
-      <rgbColor rgb="FFB3B3B3"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF004586"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
@@ -376,46 +358,12 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr b="0" sz="1400" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
-              </a:rPr>
-              <a:t>Moment</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:scatterChart>
         <c:scatterStyle val="line"/>
@@ -423,24 +371,13 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>curve1!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Moment</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="4472c4"/>
+              <a:srgbClr val="004586"/>
             </a:solidFill>
-            <a:ln w="19080">
+            <a:ln w="28800">
               <a:solidFill>
-                <a:srgbClr val="4472c4"/>
+                <a:srgbClr val="004586"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -455,10 +392,7 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
+                    <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
@@ -469,485 +403,330 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
-            <c:separator>; </c:separator>
+            <c:separator> </c:separator>
             <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>curve1!$A$2:$A$72</c:f>
+              <c:f>T1Ma!$A$2:$A$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="71"/>
+                <c:ptCount val="47"/>
                 <c:pt idx="0">
-                  <c:v>-0.127</c:v>
+                  <c:v>-0.139566929133858</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.124</c:v>
+                  <c:v>-0.133503937007874</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.12</c:v>
+                  <c:v>-0.12744094488189</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.116</c:v>
+                  <c:v>-0.121377952755905</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.113</c:v>
+                  <c:v>-0.115314960629921</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.109</c:v>
+                  <c:v>-0.109212598425197</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.106</c:v>
+                  <c:v>-0.103149606299213</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.102</c:v>
+                  <c:v>-0.0970866141732283</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.098</c:v>
+                  <c:v>-0.0910236220472441</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.095</c:v>
+                  <c:v>-0.0849606299212598</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.091</c:v>
+                  <c:v>-0.0788976377952756</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.087</c:v>
+                  <c:v>-0.0728346456692913</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-0.084</c:v>
+                  <c:v>-0.0667716535433071</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.08</c:v>
+                  <c:v>-0.0606692913385827</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-0.076</c:v>
+                  <c:v>-0.0546062992125984</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.073</c:v>
+                  <c:v>-0.0485433070866142</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-0.069</c:v>
+                  <c:v>-0.0424803149606299</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-0.065</c:v>
+                  <c:v>-0.0364173228346457</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-0.062</c:v>
+                  <c:v>-0.0303543307086614</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-0.058</c:v>
+                  <c:v>-0.0242913385826772</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-0.055</c:v>
+                  <c:v>-0.0181889763779528</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-0.051</c:v>
+                  <c:v>-0.0121259842519685</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-0.047</c:v>
+                  <c:v>-0.00606299212598425</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-0.044</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-0.04</c:v>
+                  <c:v>0.00562992125984252</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-0.036</c:v>
+                  <c:v>0.011259842519685</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-0.033</c:v>
+                  <c:v>0.0168897637795276</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-0.029</c:v>
+                  <c:v>0.0225196850393701</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-0.025</c:v>
+                  <c:v>0.0281496062992126</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-0.022</c:v>
+                  <c:v>0.0337795275590551</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-0.018</c:v>
+                  <c:v>0.0394094488188976</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-0.015</c:v>
+                  <c:v>0.0450393700787402</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-0.011</c:v>
+                  <c:v>0.0506692913385827</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-0.007</c:v>
+                  <c:v>0.0562992125984252</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-0.004</c:v>
+                  <c:v>0.0619291338582677</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0</c:v>
+                  <c:v>0.0675590551181102</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.002</c:v>
+                  <c:v>0.0731889763779527</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.005</c:v>
+                  <c:v>0.0788188976377953</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.007</c:v>
+                  <c:v>0.0844488188976378</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.01</c:v>
+                  <c:v>0.0900787401574803</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.012</c:v>
+                  <c:v>0.0957086614173228</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.014</c:v>
+                  <c:v>0.101338582677165</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.017</c:v>
+                  <c:v>0.106968503937008</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.019</c:v>
+                  <c:v>0.11259842519685</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.022</c:v>
+                  <c:v>0.118228346456693</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.024</c:v>
+                  <c:v>0.123858267716535</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.027</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>0.029</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>0.031</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>0.034</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>0.036</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>0.039</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>0.041</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>0.043</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>0.046</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>0.048</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>0.051</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>0.053</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>0.056</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>0.058</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>0.06</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>0.063</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>0.065</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>0.068</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>0.07</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>0.072</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>0.075</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>0.077</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>0.08</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>0.082</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>0.084</c:v>
+                  <c:v>0.129488188976378</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>curve1!$B$2:$B$72</c:f>
+              <c:f>T1Ma!$B$2:$B$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="71"/>
+                <c:ptCount val="47"/>
                 <c:pt idx="0">
-                  <c:v>-1.2655129</c:v>
+                  <c:v>-1.6823440984496</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.253814134</c:v>
+                  <c:v>-1.7377066644832</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1.230950386</c:v>
+                  <c:v>-1.6981619744592</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.287264598</c:v>
+                  <c:v>-1.7783812027936</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1.271829344</c:v>
+                  <c:v>-1.6992918227456</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-1.320136796</c:v>
+                  <c:v>-1.7184992436144</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-1.138605754</c:v>
+                  <c:v>-1.3343508262384</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-1.25350276</c:v>
+                  <c:v>-1.604384566688</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-1.186201494</c:v>
+                  <c:v>-1.5354638212176</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-1.296294444</c:v>
+                  <c:v>-1.4315177788688</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-1.29798476</c:v>
+                  <c:v>-1.3185329502288</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-1.169387298</c:v>
+                  <c:v>-0.971669526304</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-1.1276187</c:v>
+                  <c:v>-1.2473525081856</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-1.23370827</c:v>
+                  <c:v>-0.9129174154112</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-0.987678328</c:v>
+                  <c:v>-0.8891906013968</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-1.187713882</c:v>
+                  <c:v>-0.9852277057408</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-1.04399254</c:v>
+                  <c:v>-0.64966276468</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-0.870156884</c:v>
+                  <c:v>-0.4654974939968</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-0.88585903</c:v>
+                  <c:v>-0.4654974939968</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-1.05155448</c:v>
+                  <c:v>-0.3604216033616</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-0.853031314</c:v>
+                  <c:v>-0.5039123357344</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-0.825719366</c:v>
+                  <c:v>-0.163828001528</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-0.728081376</c:v>
+                  <c:v>-0.08473862148</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-0.844223878</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-0.614029528</c:v>
+                  <c:v>13.7513834937744</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-0.61296196</c:v>
+                  <c:v>20.3304900654816</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-0.56203007</c:v>
+                  <c:v>20.4028003558112</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-0.453138134</c:v>
+                  <c:v>20.6411983442416</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-0.305057556</c:v>
+                  <c:v>20.7191578760032</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-0.422178662</c:v>
+                  <c:v>20.8219740700656</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-0.182643092</c:v>
+                  <c:v>21.0784496310784</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-0.212801888</c:v>
+                  <c:v>20.9394782918512</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-0.214225312</c:v>
+                  <c:v>20.9089723881184</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-0.178105928</c:v>
+                  <c:v>21.2682641431936</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-0.097682472</c:v>
+                  <c:v>21.060372058496</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0</c:v>
+                  <c:v>21.1631882525584</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>6.07223782</c:v>
+                  <c:v>20.9722438921568</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>12.078375388</c:v>
+                  <c:v>21.2287194531696</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>18.011162138</c:v>
+                  <c:v>21.3631713992512</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>21.66162195</c:v>
+                  <c:v>21.2682641431936</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>21.833011096</c:v>
+                  <c:v>21.2852118674896</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>22.035181786</c:v>
+                  <c:v>21.1597987076992</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>22.029666018</c:v>
+                  <c:v>21.3755997304016</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>22.17049603</c:v>
+                  <c:v>21.3609117026784</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>22.281389656</c:v>
+                  <c:v>21.229849301456</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>22.153414942</c:v>
+                  <c:v>21.2095120323008</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>22.246827142</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>22.282501706</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>22.430849176</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>22.504288958</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>22.273116004</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>22.46363241</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>22.387256816</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>22.462031058</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>22.536716336</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>22.57061162</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>22.555398776</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>22.504377922</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>22.423865502</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>22.498372852</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>22.351359842</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>22.4789787</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>22.5212366</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>22.499707312</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>22.423465164</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>22.336280444</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>22.32951918</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>22.343886866</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>22.475153248</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>22.413456714</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>22.351404324</c:v>
+                  <c:v>21.2660044466208</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="42797145"/>
-        <c:axId val="46021323"/>
+        <c:axId val="343000"/>
+        <c:axId val="46983536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="42797145"/>
+        <c:axId val="343000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9360">
-              <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="9360">
+          <a:ln>
             <a:solidFill>
-              <a:srgbClr val="bfbfbf"/>
+              <a:srgbClr val="b3b3b3"/>
             </a:solidFill>
-            <a:round/>
           </a:ln>
         </c:spPr>
         <c:txPr>
@@ -955,21 +734,18 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46021323"/>
+        <c:crossAx val="46983536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="46021323"/>
+        <c:axId val="46983536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -977,24 +753,22 @@
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
-            <a:ln w="9360">
+            <a:ln>
               <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
+                <a:srgbClr val="b3b3b3"/>
               </a:solidFill>
-              <a:round/>
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="9360">
+          <a:ln>
             <a:solidFill>
-              <a:srgbClr val="bfbfbf"/>
+              <a:srgbClr val="b3b3b3"/>
             </a:solidFill>
-            <a:round/>
           </a:ln>
         </c:spPr>
         <c:txPr>
@@ -1002,44 +776,61 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="595959"/>
-                </a:solidFill>
-                <a:latin typeface="Calibri"/>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42797145"/>
+        <c:crossAx val="343000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
         </a:ln>
       </c:spPr>
-    </c:plotArea>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
+    <c:dispBlanksAs val="span"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
     <a:ln w="9360">
-      <a:solidFill>
-        <a:srgbClr val="d9d9d9"/>
-      </a:solidFill>
-      <a:round/>
+      <a:noFill/>
     </a:ln>
   </c:spPr>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1155,11 +946,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="7009857"/>
-        <c:axId val="73717957"/>
+        <c:axId val="42472807"/>
+        <c:axId val="30438228"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="7009857"/>
+        <c:axId val="42472807"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1187,12 +978,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73717957"/>
+        <c:crossAx val="30438228"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73717957"/>
+        <c:axId val="30438228"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1229,7 +1020,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7009857"/>
+        <c:crossAx val="42472807"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1281,25 +1072,25 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>612360</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>27360</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>36360</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>36000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>127440</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>105840</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>120600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name="Chart 1"/>
+        <xdr:cNvPr id="0" name=""/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3764160" y="728280"/>
-        <a:ext cx="8674560" cy="5893200"/>
+        <a:off x="1663200" y="210960"/>
+        <a:ext cx="5763240" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1323,9 +1114,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>28080</xdr:colOff>
+      <xdr:colOff>27360</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>143280</xdr:rowOff>
+      <xdr:rowOff>142560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1334,7 +1125,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="3241080" y="147240"/>
-        <a:ext cx="5755680" cy="3234240"/>
+        <a:ext cx="5754960" cy="3233520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1354,8 +1145,8 @@
   </sheetPr>
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1543,702 +1334,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B36"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>0.000238545613789663</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>2.39911311757586</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>0.000715454374045847</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>6.88176156994885</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>0.00121346852134564</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>8.74464902410394</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>0.00164010753407577</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>10.1024270586876</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>0.00204620237207661</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>11.5778080603252</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>0.00261907229467674</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>12.9714604390303</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>0.0033022241616947</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <v>14.3518585049475</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>0.00361371322960455</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <v>15.0353227772536</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
-        <v>0.00396533532432687</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <v>15.7456248175732</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <v>0.00430690480558074</v>
-      </c>
-      <c r="B12" s="0" t="n">
-        <v>16.4291270678529</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
-        <v>0.00466861822730222</v>
-      </c>
-      <c r="B13" s="0" t="n">
-        <v>17.2064095942861</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
-        <v>0.0050020411776572</v>
-      </c>
-      <c r="B14" s="0" t="n">
-        <v>17.8673660847904</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
-        <v>0.00539480031567431</v>
-      </c>
-      <c r="B15" s="0" t="n">
-        <v>18.5371316347184</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
-        <v>0.00578764356229404</v>
-      </c>
-      <c r="B16" s="0" t="n">
-        <v>19.2941933350847</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
-        <v>0.00626752519452117</v>
-      </c>
-      <c r="B17" s="0" t="n">
-        <v>19.9495195406586</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
-        <v>0.00667120443277795</v>
-      </c>
-      <c r="B18" s="0" t="n">
-        <v>20.6483975591559</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
-        <v>0.00710760191745247</v>
-      </c>
-      <c r="B19" s="0" t="n">
-        <v>21.3909649081419</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
-        <v>0.0076200335788921</v>
-      </c>
-      <c r="B20" s="0" t="n">
-        <v>21.9153881433281</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
-        <v>0.00814344141297315</v>
-      </c>
-      <c r="B21" s="0" t="n">
-        <v>22.5271212807089</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
-        <v>0.00862318286419592</v>
-      </c>
-      <c r="B22" s="0" t="n">
-        <v>23.0369539022191</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
-        <v>0.00908112616924064</v>
-      </c>
-      <c r="B23" s="0" t="n">
-        <v>23.5322096618098</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
-        <v>0.00939715022547084</v>
-      </c>
-      <c r="B24" s="0" t="n">
-        <v>23.6926514052193</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
-        <v>0.00996359362789055</v>
-      </c>
-      <c r="B25" s="0" t="n">
-        <v>23.7515639301842</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
-        <v>0.0106824137820501</v>
-      </c>
-      <c r="B26" s="0" t="n">
-        <v>23.6942741124895</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
-        <v>0.0115211587854399</v>
-      </c>
-      <c r="B27" s="0" t="n">
-        <v>23.7535304313677</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
-        <v>0.0123054154324349</v>
-      </c>
-      <c r="B28" s="0" t="n">
-        <v>23.7836192746504</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
-        <v>0.0129154551272107</v>
-      </c>
-      <c r="B29" s="0" t="n">
-        <v>23.8716855234542</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
-        <v>0.0142007327018904</v>
-      </c>
-      <c r="B30" s="0" t="n">
-        <v>23.8878575891308</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
-        <v>0.0158346824887158</v>
-      </c>
-      <c r="B31" s="0" t="n">
-        <v>24.0354139366737</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="n">
-        <v>0.0170436735608225</v>
-      </c>
-      <c r="B32" s="0" t="n">
-        <v>24.0078416648355</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="n">
-        <v>0.0178870892204388</v>
-      </c>
-      <c r="B33" s="0" t="n">
-        <v>24.137225371473</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="n">
-        <v>0.0194939268792614</v>
-      </c>
-      <c r="B34" s="0" t="n">
-        <v>24.1708177881311</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="n">
-        <v>0.0204391380243655</v>
-      </c>
-      <c r="B35" s="0" t="n">
-        <v>24.2035748693838</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B28"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>0.000131455399061033</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>2.40841163049727</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>0.000328638497652582</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>4.22240864831847</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>0.000492957746478873</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>6.22415573799943</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>0.000624413145539907</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>7.31878682811152</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>0.000788732394366198</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>8.3195135096292</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>0.00154460093896714</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>10.2576394078758</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>0.00207042253521127</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <v>12.0397670846507</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>0.00246478873239437</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <v>13.1964919876401</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
-        <v>0.00292488262910798</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <v>13.97771674691</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <v>0.00384507042253521</v>
-      </c>
-      <c r="B12" s="0" t="n">
-        <v>15.5714481532049</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
-        <v>0.00489671361502348</v>
-      </c>
-      <c r="B13" s="0" t="n">
-        <v>17.3213540169589</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
-        <v>0.00581690140845071</v>
-      </c>
-      <c r="B14" s="0" t="n">
-        <v>18.8212397599885</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
-        <v>0.00653990610328639</v>
-      </c>
-      <c r="B15" s="0" t="n">
-        <v>19.9773772096867</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
-        <v>0.00723004694835681</v>
-      </c>
-      <c r="B16" s="0" t="n">
-        <v>21.2899828434895</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
-        <v>0.00772300469483568</v>
-      </c>
-      <c r="B17" s="0" t="n">
-        <v>22.1649945206956</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
-        <v>0.00884037558685446</v>
-      </c>
-      <c r="B18" s="0" t="n">
-        <v>22.2568428427709</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
-        <v>0.011075117370892</v>
-      </c>
-      <c r="B19" s="0" t="n">
-        <v>22.3154119359011</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
-        <v>0.0124882629107981</v>
-      </c>
-      <c r="B20" s="0" t="n">
-        <v>22.3441677745041</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
-        <v>0.0140985915492958</v>
-      </c>
-      <c r="B21" s="0" t="n">
-        <v>22.4351349166427</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
-        <v>0.0158732394366197</v>
-      </c>
-      <c r="B22" s="0" t="n">
-        <v>22.5258083321357</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
-        <v>0.0175164319248826</v>
-      </c>
-      <c r="B23" s="0" t="n">
-        <v>22.6479986167002</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
-        <v>0.0189953051643192</v>
-      </c>
-      <c r="B24" s="0" t="n">
-        <v>22.676636964645</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
-        <v>0.0209671361502347</v>
-      </c>
-      <c r="B25" s="0" t="n">
-        <v>22.7356760204082</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
-        <v>0.0232018779342723</v>
-      </c>
-      <c r="B26" s="0" t="n">
-        <v>22.8568088890486</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
-        <v>0.025075117370892</v>
-      </c>
-      <c r="B27" s="0" t="n">
-        <v>22.9473060685541</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B9"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>6.57276995305167E-005</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>1.84545514156367</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>0.000295774647887324</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>4.06605795487208</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>0.00055868544600939</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>6.19275635958609</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>0.00055868544600939</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>6.78711222693302</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>0.00256338028169014</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>7.4091665169589</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>0.00798591549295775</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>22.258370221328</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>0.0249765258215962</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <v>23.0100460800517</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -2246,7 +1341,7 @@
   </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2586,7 +1681,7 @@
   </sheetPr>
   <dimension ref="A1:K1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2657,7 +1752,7 @@
   </sheetPr>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2916,10 +2011,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D35" activeCellId="0" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2940,7 +2035,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
@@ -2952,6 +2047,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2970,8 +2066,8 @@
   </sheetPr>
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3070,8 +2166,8 @@
   </sheetPr>
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N18" activeCellId="0" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3174,16 +2270,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F82"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.7"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -3195,590 +2288,387 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>-0.127</v>
+        <v>-0.139566929133858</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>-1.2655129</v>
+        <v>-1.6823440984496</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>-0.124</v>
+        <v>-0.133503937007874</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>-1.253814134</v>
+        <v>-1.7377066644832</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>-0.12</v>
+        <v>-0.12744094488189</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>-1.230950386</v>
+        <v>-1.6981619744592</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>-0.116</v>
+        <v>-0.121377952755905</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>-1.287264598</v>
+        <v>-1.7783812027936</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>-0.113</v>
+        <v>-0.115314960629921</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>-1.271829344</v>
+        <v>-1.6992918227456</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>-0.109</v>
+        <v>-0.109212598425197</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>-1.320136796</v>
+        <v>-1.7184992436144</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>-0.106</v>
+        <v>-0.103149606299213</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>-1.138605754</v>
+        <v>-1.3343508262384</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>-0.102</v>
+        <v>-0.0970866141732283</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>-1.25350276</v>
+        <v>-1.604384566688</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>-0.098</v>
+        <v>-0.0910236220472441</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>-1.186201494</v>
+        <v>-1.5354638212176</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>-0.095</v>
+        <v>-0.0849606299212598</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>-1.296294444</v>
+        <v>-1.4315177788688</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>-0.091</v>
+        <v>-0.0788976377952756</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>-1.29798476</v>
+        <v>-1.3185329502288</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>-0.087</v>
+        <v>-0.0728346456692913</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>-1.169387298</v>
+        <v>-0.971669526304</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>-0.084</v>
+        <v>-0.0667716535433071</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>-1.1276187</v>
+        <v>-1.2473525081856</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="n">
-        <v>-0.08</v>
+      <c r="A15" s="0" t="n">
+        <v>-0.0606692913385827</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>-1.23370827</v>
+        <v>-0.9129174154112</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="n">
-        <v>-0.076</v>
+      <c r="A16" s="0" t="n">
+        <v>-0.0546062992125984</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>-0.987678328</v>
+        <v>-0.8891906013968</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="n">
-        <v>-0.073</v>
+      <c r="A17" s="0" t="n">
+        <v>-0.0485433070866142</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>-1.187713882</v>
+        <v>-0.9852277057408</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="n">
-        <v>-0.069</v>
+      <c r="A18" s="0" t="n">
+        <v>-0.0424803149606299</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>-1.04399254</v>
+        <v>-0.64966276468</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="n">
-        <v>-0.065</v>
+      <c r="A19" s="0" t="n">
+        <v>-0.0364173228346457</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>-0.870156884</v>
+        <v>-0.4654974939968</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="n">
-        <v>-0.062</v>
+      <c r="A20" s="0" t="n">
+        <v>-0.0303543307086614</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>-0.88585903</v>
+        <v>-0.4654974939968</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="n">
-        <v>-0.058</v>
+      <c r="A21" s="0" t="n">
+        <v>-0.0242913385826772</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>-1.05155448</v>
+        <v>-0.3604216033616</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="n">
-        <v>-0.055</v>
+      <c r="A22" s="0" t="n">
+        <v>-0.0181889763779528</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>-0.853031314</v>
+        <v>-0.5039123357344</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="n">
-        <v>-0.051</v>
+      <c r="A23" s="0" t="n">
+        <v>-0.0121259842519685</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>-0.825719366</v>
+        <v>-0.163828001528</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="n">
-        <v>-0.047</v>
+      <c r="A24" s="0" t="n">
+        <v>-0.00606299212598425</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>-0.728081376</v>
+        <v>-0.08473862148</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="n">
-        <v>-0.044</v>
+      <c r="A25" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>-0.844223878</v>
-      </c>
-      <c r="F25" s="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>-0.04</v>
+        <v>0.00562992125984252</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>-0.614029528</v>
+        <v>13.7513834937744</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>-0.036</v>
+        <v>0.011259842519685</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>-0.61296196</v>
+        <v>20.3304900654816</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>-0.033</v>
+        <v>0.0168897637795276</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>-0.56203007</v>
+        <v>20.4028003558112</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="n">
-        <v>-0.029</v>
+      <c r="A29" s="0" t="n">
+        <v>0.0225196850393701</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>-0.453138134</v>
+        <v>20.6411983442416</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3" t="n">
-        <v>-0.025</v>
+      <c r="A30" s="0" t="n">
+        <v>0.0281496062992126</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>-0.305057556</v>
+        <v>20.7191578760032</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="n">
-        <v>-0.022</v>
+      <c r="A31" s="0" t="n">
+        <v>0.0337795275590551</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>-0.422178662</v>
+        <v>20.8219740700656</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
-        <v>-0.018</v>
+        <v>0.0394094488188976</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>-0.182643092</v>
+        <v>21.0784496310784</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
-        <v>-0.015</v>
+        <v>0.0450393700787402</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>-0.212801888</v>
+        <v>20.9394782918512</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
-        <v>-0.011</v>
+        <v>0.0506692913385827</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>-0.214225312</v>
+        <v>20.9089723881184</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
-        <v>-0.007</v>
+        <v>0.0562992125984252</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>-0.178105928</v>
+        <v>21.2682641431936</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
-        <v>-0.004</v>
+        <v>0.0619291338582677</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>-0.097682472</v>
+        <v>21.060372058496</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
-        <v>0</v>
+        <v>0.0675590551181102</v>
       </c>
       <c r="B37" s="0" t="n">
-        <v>0</v>
+        <v>21.1631882525584</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
-        <v>0.002</v>
+        <v>0.0731889763779527</v>
       </c>
       <c r="B38" s="0" t="n">
-        <v>6.07223782</v>
+        <v>20.9722438921568</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
-        <v>0.005</v>
+        <v>0.0788188976377953</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>12.078375388</v>
+        <v>21.2287194531696</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
-        <v>0.007</v>
+        <v>0.0844488188976378</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>18.011162138</v>
+        <v>21.3631713992512</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
-        <v>0.01</v>
+        <v>0.0900787401574803</v>
       </c>
       <c r="B41" s="0" t="n">
-        <v>21.66162195</v>
+        <v>21.2682641431936</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
-        <v>0.012</v>
+        <v>0.0957086614173228</v>
       </c>
       <c r="B42" s="0" t="n">
-        <v>21.833011096</v>
+        <v>21.2852118674896</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
-        <v>0.014</v>
+        <v>0.101338582677165</v>
       </c>
       <c r="B43" s="0" t="n">
-        <v>22.035181786</v>
+        <v>21.1597987076992</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
-        <v>0.017</v>
+        <v>0.106968503937008</v>
       </c>
       <c r="B44" s="0" t="n">
-        <v>22.029666018</v>
+        <v>21.3755997304016</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
-        <v>0.019</v>
+        <v>0.11259842519685</v>
       </c>
       <c r="B45" s="0" t="n">
-        <v>22.17049603</v>
+        <v>21.3609117026784</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
-        <v>0.022</v>
+        <v>0.118228346456693</v>
       </c>
       <c r="B46" s="0" t="n">
-        <v>22.281389656</v>
+        <v>21.229849301456</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
-        <v>0.024</v>
+        <v>0.123858267716535</v>
       </c>
       <c r="B47" s="0" t="n">
-        <v>22.153414942</v>
+        <v>21.2095120323008</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
-        <v>0.027</v>
+        <v>0.129488188976378</v>
       </c>
       <c r="B48" s="0" t="n">
-        <v>22.246827142</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="n">
-        <v>0.029</v>
-      </c>
-      <c r="B49" s="0" t="n">
-        <v>22.282501706</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="n">
-        <v>0.031</v>
-      </c>
-      <c r="B50" s="0" t="n">
-        <v>22.430849176</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="n">
-        <v>0.034</v>
-      </c>
-      <c r="B51" s="0" t="n">
-        <v>22.504288958</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="n">
-        <v>0.036</v>
-      </c>
-      <c r="B52" s="0" t="n">
-        <v>22.273116004</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="n">
-        <v>0.039</v>
-      </c>
-      <c r="B53" s="0" t="n">
-        <v>22.46363241</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="n">
-        <v>0.041</v>
-      </c>
-      <c r="B54" s="0" t="n">
-        <v>22.387256816</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="n">
-        <v>0.043</v>
-      </c>
-      <c r="B55" s="0" t="n">
-        <v>22.462031058</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="n">
-        <v>0.046</v>
-      </c>
-      <c r="B56" s="0" t="n">
-        <v>22.536716336</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="n">
-        <v>0.048</v>
-      </c>
-      <c r="B57" s="0" t="n">
-        <v>22.57061162</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="n">
-        <v>0.051</v>
-      </c>
-      <c r="B58" s="0" t="n">
-        <v>22.555398776</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="n">
-        <v>0.053</v>
-      </c>
-      <c r="B59" s="0" t="n">
-        <v>22.504377922</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="n">
-        <v>0.056</v>
-      </c>
-      <c r="B60" s="0" t="n">
-        <v>22.423865502</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="n">
-        <v>0.058</v>
-      </c>
-      <c r="B61" s="0" t="n">
-        <v>22.498372852</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="B62" s="0" t="n">
-        <v>22.351359842</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="n">
-        <v>0.063</v>
-      </c>
-      <c r="B63" s="0" t="n">
-        <v>22.4789787</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="n">
-        <v>0.065</v>
-      </c>
-      <c r="B64" s="0" t="n">
-        <v>22.5212366</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="n">
-        <v>0.068</v>
-      </c>
-      <c r="B65" s="0" t="n">
-        <v>22.499707312</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="B66" s="0" t="n">
-        <v>22.423465164</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="n">
-        <v>0.072</v>
-      </c>
-      <c r="B67" s="0" t="n">
-        <v>22.336280444</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="n">
-        <v>0.075</v>
-      </c>
-      <c r="B68" s="0" t="n">
-        <v>22.32951918</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="n">
-        <v>0.077</v>
-      </c>
-      <c r="B69" s="0" t="n">
-        <v>22.343886866</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="B70" s="0" t="n">
-        <v>22.475153248</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="n">
-        <v>0.082</v>
-      </c>
-      <c r="B71" s="0" t="n">
-        <v>22.413456714</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="n">
-        <v>0.084</v>
-      </c>
-      <c r="B72" s="0" t="n">
-        <v>22.351404324</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>21.2660044466208</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -3791,7 +2681,7 @@
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -3799,10 +2689,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>